<commit_message>
modifica k means, risoluzione bug con le combinazioni. Split train test non random ma sequenziale. Aggiunta split sequenziale anche in tfidf (>0.8)
</commit_message>
<xml_diff>
--- a/performance_ML.xlsx
+++ b/performance_ML.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonemalesardi/Documents/Università/Retrieval/The-winner-of-the-next-game/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0033604-696E-864D-93EE-49A07FB86FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3DB1215-CA49-704E-B933-CD0F03C8EEA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3600" windowWidth="38400" windowHeight="21600" xr2:uid="{EEB7B157-5F71-AD42-AF60-64C8E20BEB1C}"/>
+    <workbookView xWindow="-38400" yWindow="-3600" windowWidth="38400" windowHeight="21600" activeTab="7" xr2:uid="{EEB7B157-5F71-AD42-AF60-64C8E20BEB1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Logistic Regression" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,10 @@
     <sheet name="Random Forest" sheetId="5" r:id="rId5"/>
     <sheet name="K-Nearest Neighbors" sheetId="6" r:id="rId6"/>
     <sheet name="Refs" sheetId="9" r:id="rId7"/>
+    <sheet name="Tokenizzazione" sheetId="10" r:id="rId8"/>
+    <sheet name="K-means" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="122">
   <si>
     <t xml:space="preserve">Approccio </t>
   </si>
@@ -325,13 +327,103 @@
     <t>• bi-gram
 • TfIdfVectorizer
 • conversione squadre</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/python-nlp-analysis-of-restaurant-reviews/</t>
+  </si>
+  <si>
+    <t>Tokenizzazione</t>
+  </si>
+  <si>
+    <t>word_tokenize</t>
+  </si>
+  <si>
+    <t>Stemming</t>
+  </si>
+  <si>
+    <t>PorterStemmer()</t>
+  </si>
+  <si>
+    <t>RegexpTokenizer</t>
+  </si>
+  <si>
+    <t>spacy</t>
+  </si>
+  <si>
+    <t>lemmatization</t>
+  </si>
+  <si>
+    <t>Logistic Regression</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>Multinomial Naive Bayes</t>
+  </si>
+  <si>
+    <t>Decision Tree</t>
+  </si>
+  <si>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>K-Nearest Neighbors</t>
+  </si>
+  <si>
+    <t>regex</t>
+  </si>
+  <si>
+    <t>word tokenize</t>
+  </si>
+  <si>
+    <t>spacy lemmatization</t>
+  </si>
+  <si>
+    <t>spacy stemmer</t>
+  </si>
+  <si>
+    <t>accuratezza (min 0,76)</t>
+  </si>
+  <si>
+    <t>CountVectorizer</t>
+  </si>
+  <si>
+    <t>sklearn</t>
+  </si>
+  <si>
+    <t>test size = 0,2</t>
+  </si>
+  <si>
+    <t>test size = 0,3</t>
+  </si>
+  <si>
+    <t>tempo (s)</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>TfIdf</t>
+  </si>
+  <si>
+    <t>&gt;= 0,76</t>
+  </si>
+  <si>
+    <t>&gt;= 0,79</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>?? = interrotto dopo lungo tempo di esecuzione</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -383,8 +475,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -401,6 +501,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -526,7 +638,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -606,6 +718,25 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -924,7 +1055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1C3E033-4B37-DE4D-AD4B-FF1BCF73E02B}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1707,10 +1838,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C5FC4D-C604-284D-9D39-16EDC76666DD}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="135" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1759,12 +1890,423 @@
         <v>90</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" s="30" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{01ECCFF3-B4F6-2F4A-B390-B9A719B2343E}"/>
     <hyperlink ref="B3:B4" r:id="rId2" display="https://www.datacamp.com/tutorial/text-analytics-beginners-nltk" xr:uid="{37BF0218-FC56-C644-A9F4-5C68C8E05B05}"/>
     <hyperlink ref="B5" r:id="rId3" xr:uid="{0ED097BE-B910-2B4D-AA88-2F25A50DA326}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{FB987821-1A80-EC43-97A1-2037D9F36BB7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B345EB28-290F-F34E-A159-605E92B2B2A1}">
+  <dimension ref="A1:I30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26:E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" s="31"/>
+      <c r="I2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="31"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="31"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F5" s="31"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" s="35">
+        <v>0.763158</v>
+      </c>
+      <c r="C12" s="36">
+        <v>0.77193000000000001</v>
+      </c>
+      <c r="D12" s="36">
+        <v>0.80263200000000001</v>
+      </c>
+      <c r="E12" s="36">
+        <v>0.79824600000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="36">
+        <v>2.8</v>
+      </c>
+      <c r="C13" s="36">
+        <v>3.4</v>
+      </c>
+      <c r="D13" s="36">
+        <v>1.3</v>
+      </c>
+      <c r="E13" s="36">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C15" s="32"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" s="35"/>
+      <c r="C17" s="36">
+        <v>0.77193000000000001</v>
+      </c>
+      <c r="D17" s="36">
+        <v>0.80263200000000001</v>
+      </c>
+      <c r="E17" s="36">
+        <v>0.79824600000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36">
+        <v>1.7</v>
+      </c>
+      <c r="D18" s="36">
+        <v>0.2</v>
+      </c>
+      <c r="E18" s="36">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" s="36" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" s="34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="B22" s="35">
+        <v>0.763158</v>
+      </c>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="E22" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="H22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B23" s="36">
+        <v>12.2</v>
+      </c>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="E23" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="F23" s="37"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" s="36" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" s="34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="B27" s="35">
+        <v>0.763158</v>
+      </c>
+      <c r="C27" s="36">
+        <v>0.77193000000000001</v>
+      </c>
+      <c r="D27" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="E27" s="36" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28" s="35">
+        <v>0.9</v>
+      </c>
+      <c r="C28" s="36">
+        <v>1.7</v>
+      </c>
+      <c r="D28" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="E28" s="36" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="B29" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" s="36" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871DE84F-8B3C-AF41-AB6D-0D94A5BF0E68}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>